<commit_message>
Participants DONE plus sports start
Sports isnt final at all, should duplicate for the medals id and stuff, sport id is only eliminating duplicates.
</commit_message>
<xml_diff>
--- a/dataset/new_datasets/DummyExcel.xlsx
+++ b/dataset/new_datasets/DummyExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\uni\BD\dataset\new_datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53733C11-4060-4F3B-9D1B-9892F697CC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA98476-C21A-4296-9A27-81265144D604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10420" yWindow="11210" windowWidth="8910" windowHeight="10610" xr2:uid="{39355EEB-7048-4A6D-B52D-A6434C8288CC}"/>
+    <workbookView minimized="1" xWindow="820" yWindow="11550" windowWidth="19430" windowHeight="10610" xr2:uid="{39355EEB-7048-4A6D-B52D-A6434C8288CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>athlete_url</t>
   </si>
@@ -106,10 +106,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,13 +140,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D30C8D6-7E7C-4889-A3BF-4A55FC0A4901}">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +473,7 @@
     <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,23 +489,8 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -510,23 +506,8 @@
       <c r="E2">
         <v>3</v>
       </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2">
-        <v>1992</v>
-      </c>
-      <c r="N2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -542,23 +523,8 @@
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="J3" t="s">
-        <v>5</v>
-      </c>
-      <c r="O3">
-        <v>4461</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -574,24 +540,9 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4">
-        <v>1997</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F5">
@@ -606,23 +557,8 @@
       <c r="I5">
         <v>1</v>
       </c>
-      <c r="J5" t="s">
-        <v>8</v>
-      </c>
-      <c r="O5">
-        <v>2175</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -635,20 +571,8 @@
       <c r="D6">
         <v>1987</v>
       </c>
-      <c r="J6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6">
-        <v>1987</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -664,23 +588,8 @@
       <c r="I7">
         <v>0</v>
       </c>
-      <c r="J7" t="s">
-        <v>11</v>
-      </c>
-      <c r="O7">
-        <v>189</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -696,23 +605,8 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="J8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" t="s">
-        <v>10</v>
-      </c>
-      <c r="M8">
-        <v>1986</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -728,23 +622,8 @@
       <c r="I9">
         <v>0</v>
       </c>
-      <c r="J9" t="s">
-        <v>13</v>
-      </c>
-      <c r="O9">
-        <v>957</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -760,23 +639,8 @@
       <c r="E10">
         <v>2</v>
       </c>
-      <c r="J10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M10">
-        <v>1990</v>
-      </c>
-      <c r="N10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -792,23 +656,8 @@
       <c r="I11">
         <v>0</v>
       </c>
-      <c r="J11" t="s">
-        <v>15</v>
-      </c>
-      <c r="O11">
-        <v>1371</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -824,23 +673,8 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="J12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L12" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12">
-        <v>1996</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -856,23 +690,8 @@
       <c r="I13">
         <v>0</v>
       </c>
-      <c r="J13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O13">
-        <v>3385</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -888,23 +707,8 @@
       <c r="E14">
         <v>2</v>
       </c>
-      <c r="J14" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L14" t="s">
-        <v>17</v>
-      </c>
-      <c r="M14">
-        <v>1996</v>
-      </c>
-      <c r="N14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -920,28 +724,16 @@
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15" t="s">
-        <v>20</v>
-      </c>
-      <c r="O15">
-        <v>5036</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <dataConsolidate leftLabels="1" topLabels="1">
+  <dataConsolidate topLabels="1">
     <dataRefs count="1">
       <dataRef ref="A1:I11" sheet="Sheet1"/>
     </dataRefs>
   </dataConsolidate>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" xr:uid="{8E55EAA8-AA72-4C51-A88A-7CD9A5B732E7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>